<commit_message>
Fixing geopoint in shared_table model
</commit_message>
<xml_diff>
--- a/form-files/shared_table_a/shared_table_a.xlsx
+++ b/form-files/shared_table_a/shared_table_a.xlsx
@@ -97,16 +97,16 @@
     <t>schema.elementType</t>
   </si>
   <si>
-    <t>schema.properties.latitude</t>
-  </si>
-  <si>
-    <t>schema.properties.longitude</t>
-  </si>
-  <si>
-    <t>schema.properties.altitude</t>
-  </si>
-  <si>
-    <t>schema.properties.accuracy</t>
+    <t>schema.properties.latitude.type</t>
+  </si>
+  <si>
+    <t>schema.properties.longitude.type</t>
+  </si>
+  <si>
+    <t>schema.properties.altitude.type</t>
+  </si>
+  <si>
+    <t>schema.properties.accuracy.type</t>
   </si>
   <si>
     <t>string</t>

</xml_diff>